<commit_message>
changed Backlog and Burndown chart
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint4/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint4/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhertz/Documents/subjects/SE/ganttproject/Project/Phase 2/Sprint4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D6303A-F1E3-164C-B9FD-7EB1C0FDAD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1CF6CA-9EA1-5A42-864D-DC06B1DE74AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="560" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -60,13 +60,13 @@
     <t>Implement feature 1 (Ricardo)</t>
   </si>
   <si>
-    <t>Upload sprints to github (Todo mundo)</t>
+    <t>Implement feature 2 (James, João, Francisco, Iago)</t>
   </si>
   <si>
-    <t>Take metrics (João)</t>
+    <t>Upload sprints to github (Todo agente)</t>
   </si>
   <si>
-    <t>Implement feature 2 (James, João, Francisco, Iago)</t>
+    <t>Take metrics (Toda agente)</t>
   </si>
 </sst>
 </file>
@@ -2222,7 +2222,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="23">
         <v>5</v>
@@ -2246,7 +2246,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="23">
         <v>2</v>
@@ -2268,7 +2268,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="23">
         <v>1</v>

</xml_diff>

<commit_message>
uploaded work breakdown structure
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint4/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint4/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhertz/Documents/subjects/SE/ganttproject/Project/Phase 2/Sprint4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1CF6CA-9EA1-5A42-864D-DC06B1DE74AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA531890-423D-2C4E-9DA5-F6AFA3FD05FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,16 +693,16 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,13 +818,13 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2094,7 +2094,7 @@
   <dimension ref="B1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2255,13 +2255,17 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21">
@@ -2276,14 +2280,16 @@
       <c r="E9" s="10"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="8">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="26" t="s">
@@ -2307,19 +2313,19 @@
       </c>
       <c r="H10" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="J10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L10" s="18"/>
     </row>
@@ -2346,15 +2352,15 @@
       </c>
       <c r="H11" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="J11" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="1"/>

</xml_diff>